<commit_message>
fullheight table & multiple remove
</commit_message>
<xml_diff>
--- a/packages/front/assets/import-objects-example.xlsx
+++ b/packages/front/assets/import-objects-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\rengin-erp\packages\front\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F637F2C1-068E-4EDF-AAC5-47276C74ABFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB38B782-E09F-4C82-976F-333CFE9DE4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A61CECF-C11D-4582-B265-B89C5C7357F7}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8964" xr2:uid="{1A61CECF-C11D-4582-B265-B89C5C7357F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Адрес</t>
+  </si>
+  <si>
+    <t>Город</t>
+  </si>
+  <si>
+    <t>Юр.лицо</t>
+  </si>
+  <si>
+    <t>Заказчик</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,15 +62,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Inconsolata"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -70,7 +97,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,14 +105,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,179 +446,81 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" customWidth="1"/>
     <col min="2" max="2" width="27.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("IMPORTRANGE(""https://docs.google.com/spreadsheets/d/1Ul25vXT6wrF0nA8jPwPoZBuIRWGml0IiVqoTWlYcGnA/edit?usp=sharing"",""Заказчики!A:D"")"),"Заказчик")</f>
-        <v>Заказчик</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
       </c>
-      <c r="B1" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Юр.лицо")</f>
-        <v>Юр.лицо</v>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
       </c>
-      <c r="C1" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Город")</f>
-        <v>Город</v>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
       </c>
-      <c r="D1" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Адрес")</f>
-        <v>Адрес</v>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Винлаб")</f>
-        <v>Винлаб</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"АО Винлаб Благовещенск")</f>
-        <v>АО Винлаб Благовещенск</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"п.Солнечный")</f>
-        <v>п.Солнечный</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ул.Геологов, 10")</f>
-        <v>ул.Геологов, 10</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Винлаб")</f>
-        <v>Винлаб</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"АО Винлаб Благовещенск")</f>
-        <v>АО Винлаб Благовещенск</v>
-      </c>
-      <c r="C3" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"п.Солнечный")</f>
-        <v>п.Солнечный</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ул.Геологов, 20Б")</f>
-        <v>ул.Геологов, 20Б</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Винлаб")</f>
-        <v>Винлаб</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"АО Винлаб")</f>
-        <v>АО Винлаб</v>
-      </c>
-      <c r="C4" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"г.Хабаровск")</f>
-        <v>г.Хабаровск</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ул.Флегонтова, 4")</f>
-        <v>ул.Флегонтова, 4</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Винлаб")</f>
-        <v>Винлаб</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ООО Винлаб Владивосток")</f>
-        <v>ООО Винлаб Владивосток</v>
-      </c>
-      <c r="C5" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"г.Хабаровск")</f>
-        <v>г.Хабаровск</v>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ул.Волочаевская, 21")</f>
-        <v>ул.Волочаевская, 21</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Гемотест")</f>
-        <v>Гемотест</v>
-      </c>
-      <c r="B6" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ООО Гемотест Западная сибирь ")</f>
-        <v xml:space="preserve">ООО Гемотест Западная сибирь </v>
-      </c>
-      <c r="C6" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"п. Кольцово")</f>
-        <v>п. Кольцово</v>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"пр-т Никольский, д. 15")</f>
-        <v>пр-т Никольский, д. 15</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Гемотест")</f>
-        <v>Гемотест</v>
-      </c>
-      <c r="B7" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ООО Гемотест Иркутск ")</f>
-        <v xml:space="preserve">ООО Гемотест Иркутск </v>
-      </c>
-      <c r="C7" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"г. Ангарск")</f>
-        <v>г. Ангарск</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"15-й микрорайон, 1")</f>
-        <v>15-й микрорайон, 1</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Гемотест")</f>
-        <v>Гемотест</v>
-      </c>
-      <c r="B8" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ООО Гемотест Иркутск ")</f>
-        <v xml:space="preserve">ООО Гемотест Иркутск </v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"г. Ангарск")</f>
-        <v>г. Ангарск</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"33-й микрорайон, 1")</f>
-        <v>33-й микрорайон, 1</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Гемотест")</f>
-        <v>Гемотест</v>
-      </c>
-      <c r="B9" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ООО Гемотест Иркутск ")</f>
-        <v xml:space="preserve">ООО Гемотест Иркутск </v>
-      </c>
-      <c r="C9" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"г. Ангарск")</f>
-        <v>г. Ангарск</v>
-      </c>
-      <c r="D9" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"73 квартал, 8")</f>
-        <v>73 квартал, 8</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>